<commit_message>
Updated class in testng xml
</commit_message>
<xml_diff>
--- a/test-output/TestReport.xlsx
+++ b/test-output/TestReport.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -29,10 +29,13 @@
     <t>PASSED</t>
   </si>
   <si>
-    <t>Tue Mar 25 16:11:15 IST 2025</t>
+    <t>Tue Mar 25 16:16:42 IST 2025</t>
   </si>
   <si>
     <t>Verify Home Page Loads Successfully</t>
+  </si>
+  <si>
+    <t>Tue Mar 25 16:16:43 IST 2025</t>
   </si>
 </sst>
 </file>
@@ -113,7 +116,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated report with sub-steps
</commit_message>
<xml_diff>
--- a/test-output/TestReport.xlsx
+++ b/test-output/TestReport.xlsx
@@ -12,11 +12,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="22">
   <si>
     <t>Test Case Name</t>
   </si>
   <si>
+    <t>Step Name</t>
+  </si>
+  <si>
     <t>Status</t>
   </si>
   <si>
@@ -29,10 +32,13 @@
     <t>User Login with Valid Credentials</t>
   </si>
   <si>
+    <t>No Sub-Steps</t>
+  </si>
+  <si>
     <t>PASSED</t>
   </si>
   <si>
-    <t>Thu Mar 27 12:56:16 IST 2025</t>
+    <t>Thu Mar 27 13:31:11 IST 2025</t>
   </si>
   <si>
     <t>Test executed successfully.</t>
@@ -41,7 +47,34 @@
     <t>User Login with Invalid Credentials</t>
   </si>
   <si>
-    <t>Thu Mar 27 12:56:21 IST 2025</t>
+    <t>Invalid Email Attempt</t>
+  </si>
+  <si>
+    <t>Thu Mar 27 13:31:15 IST 2025</t>
+  </si>
+  <si>
+    <t>Error displayed correctly</t>
+  </si>
+  <si>
+    <t>Clear User ID Field</t>
+  </si>
+  <si>
+    <t>Field cleared successfully</t>
+  </si>
+  <si>
+    <t>Invalid OTP Attempt</t>
+  </si>
+  <si>
+    <t>Thu Mar 27 13:31:17 IST 2025</t>
+  </si>
+  <si>
+    <t>Error displayed correctly for invalid OTP</t>
+  </si>
+  <si>
+    <t>Click 'Go to Sign In'</t>
+  </si>
+  <si>
+    <t>Navigated back to Get OTP page successfully</t>
   </si>
   <si>
     <t>Verify Home Page Loads Successfully</t>
@@ -89,7 +122,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -108,33 +141,42 @@
       <c r="D1" t="s" s="0">
         <v>3</v>
       </c>
+      <c r="E1" t="s" s="0">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>7</v>
+        <v>12</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>13</v>
       </c>
     </row>
     <row r="4">
@@ -142,13 +184,84 @@
         <v>10</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="D4" t="s" s="0">
-        <v>7</v>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated report to delete automatically
</commit_message>
<xml_diff>
--- a/test-output/TestReport.xlsx
+++ b/test-output/TestReport.xlsx
@@ -41,7 +41,7 @@
     <t>PASSED</t>
   </si>
   <si>
-    <t>03/27/2025 06:12:34 PM</t>
+    <t>03/27/2025 06:24:01 PM</t>
   </si>
   <si>
     <t>Test executed successfully.</t>
@@ -53,7 +53,7 @@
     <t>Invalid Email Attempt</t>
   </si>
   <si>
-    <t>03/27/2025 06:12:37 PM</t>
+    <t>03/27/2025 06:24:06 PM</t>
   </si>
   <si>
     <t>Error Message -&gt; Invalid email address. Please enter a valid email</t>
@@ -62,7 +62,7 @@
     <t>Not Registered Email Attempt</t>
   </si>
   <si>
-    <t>03/27/2025 06:12:38 PM</t>
+    <t>03/27/2025 06:24:07 PM</t>
   </si>
   <si>
     <t>Error Message -&gt; No such user found</t>
@@ -71,7 +71,7 @@
     <t>Invalid OTP Attempt</t>
   </si>
   <si>
-    <t>03/27/2025 06:12:40 PM</t>
+    <t>03/27/2025 06:24:09 PM</t>
   </si>
   <si>
     <t>Error Message -&gt; Incorrect OTP</t>
@@ -83,7 +83,7 @@
     <t>Navigated back to Get OTP page successfully</t>
   </si>
   <si>
-    <t>03/27/2025 06:12:41 PM</t>
+    <t>03/27/2025 06:24:10 PM</t>
   </si>
   <si>
     <t>Verify Home Page Loads Successfully</t>

</xml_diff>

<commit_message>
date format updated in the report
</commit_message>
<xml_diff>
--- a/test-output/TestReport.xlsx
+++ b/test-output/TestReport.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -41,7 +41,7 @@
     <t>PASSED</t>
   </si>
   <si>
-    <t>03/27/2025 06:24:01 PM</t>
+    <t>28/03/2025 10:42:39 AM</t>
   </si>
   <si>
     <t>Test executed successfully.</t>
@@ -53,7 +53,7 @@
     <t>Invalid Email Attempt</t>
   </si>
   <si>
-    <t>03/27/2025 06:24:06 PM</t>
+    <t>28/03/2025 10:42:43 AM</t>
   </si>
   <si>
     <t>Error Message -&gt; Invalid email address. Please enter a valid email</t>
@@ -62,7 +62,7 @@
     <t>Not Registered Email Attempt</t>
   </si>
   <si>
-    <t>03/27/2025 06:24:07 PM</t>
+    <t>28/03/2025 10:42:45 AM</t>
   </si>
   <si>
     <t>Error Message -&gt; No such user found</t>
@@ -71,7 +71,7 @@
     <t>Invalid OTP Attempt</t>
   </si>
   <si>
-    <t>03/27/2025 06:24:09 PM</t>
+    <t>28/03/2025 10:42:47 AM</t>
   </si>
   <si>
     <t>Error Message -&gt; Incorrect OTP</t>
@@ -81,9 +81,6 @@
   </si>
   <si>
     <t>Navigated back to Get OTP page successfully</t>
-  </si>
-  <si>
-    <t>03/27/2025 06:24:10 PM</t>
   </si>
   <si>
     <t>Verify Home Page Loads Successfully</t>
@@ -277,7 +274,7 @@
         <v>8</v>
       </c>
       <c r="E7" t="s" s="0">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F7" t="s" s="0">
         <v>10</v>
@@ -288,7 +285,7 @@
         <v>3.0</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s" s="0">
         <v>7</v>
@@ -297,7 +294,7 @@
         <v>8</v>
       </c>
       <c r="E8" t="s" s="0">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F8" t="s" s="0">
         <v>10</v>

</xml_diff>

<commit_message>
Added account block test case
</commit_message>
<xml_diff>
--- a/test-output/TestReport.xlsx
+++ b/test-output/TestReport.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -41,46 +41,58 @@
     <t>PASSED</t>
   </si>
   <si>
-    <t>28/03/2025 10:42:39 AM</t>
+    <t>28/03/2025 03:09:19 PM</t>
   </si>
   <si>
     <t>Test executed successfully.</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
+    <t>Invalid Email Attempt</t>
+  </si>
+  <si>
+    <t>28/03/2025 03:09:22 PM</t>
+  </si>
+  <si>
+    <t>Error Message -&gt; Invalid email address. Please enter a valid email</t>
+  </si>
+  <si>
+    <t>Not Registered Email Attempt</t>
+  </si>
+  <si>
+    <t>28/03/2025 03:09:23 PM</t>
+  </si>
+  <si>
+    <t>Error Message -&gt; No such user found</t>
+  </si>
+  <si>
+    <t>Invalid OTP Attempt</t>
+  </si>
+  <si>
+    <t>28/03/2025 03:09:25 PM</t>
+  </si>
+  <si>
+    <t>Error Message -&gt; Incorrect OTP</t>
+  </si>
+  <si>
+    <t>Account Blocked After Multiple Wrong OTPs</t>
+  </si>
+  <si>
+    <t>28/03/2025 03:09:30 PM</t>
+  </si>
+  <si>
+    <t>You have reached the maximum login attempts for the day. Please try again after 24 hours.</t>
+  </si>
+  <si>
+    <t>Click Go to Sign In</t>
+  </si>
+  <si>
+    <t>Navigated back to Get OTP page successfully</t>
+  </si>
+  <si>
     <t>User Login with Invalid Credentials</t>
-  </si>
-  <si>
-    <t>Invalid Email Attempt</t>
-  </si>
-  <si>
-    <t>28/03/2025 10:42:43 AM</t>
-  </si>
-  <si>
-    <t>Error Message -&gt; Invalid email address. Please enter a valid email</t>
-  </si>
-  <si>
-    <t>Not Registered Email Attempt</t>
-  </si>
-  <si>
-    <t>28/03/2025 10:42:45 AM</t>
-  </si>
-  <si>
-    <t>Error Message -&gt; No such user found</t>
-  </si>
-  <si>
-    <t>Invalid OTP Attempt</t>
-  </si>
-  <si>
-    <t>28/03/2025 10:42:47 AM</t>
-  </si>
-  <si>
-    <t>Error Message -&gt; Incorrect OTP</t>
-  </si>
-  <si>
-    <t>Click Go to Sign In</t>
-  </si>
-  <si>
-    <t>Navigated back to Get OTP page successfully</t>
   </si>
   <si>
     <t>Verify Home Page Loads Successfully</t>
@@ -134,7 +146,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -254,10 +266,10 @@
         <v>8</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7">
@@ -268,16 +280,16 @@
         <v>11</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s" s="0">
         <v>8</v>
       </c>
       <c r="E7" t="s" s="0">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F7" t="s" s="0">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8">
@@ -285,7 +297,7 @@
         <v>3.0</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s" s="0">
         <v>7</v>
@@ -294,9 +306,29 @@
         <v>8</v>
       </c>
       <c r="E8" t="s" s="0">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F8" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="F9" t="s" s="0">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Incomplete for step 6
</commit_message>
<xml_diff>
--- a/test-output/TestReport.xlsx
+++ b/test-output/TestReport.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -41,7 +41,7 @@
     <t>PASSED</t>
   </si>
   <si>
-    <t>28/03/2025 03:19:15 PM</t>
+    <t>28/03/2025 03:46:14 PM</t>
   </si>
   <si>
     <t>Test executed successfully.</t>
@@ -53,7 +53,7 @@
     <t>Invalid Email Attempt</t>
   </si>
   <si>
-    <t>28/03/2025 03:19:17 PM</t>
+    <t>28/03/2025 03:46:17 PM</t>
   </si>
   <si>
     <t>Error Message -&gt; Invalid email address. Please enter a valid email</t>
@@ -62,7 +62,7 @@
     <t>Not Registered Email Attempt</t>
   </si>
   <si>
-    <t>28/03/2025 03:19:19 PM</t>
+    <t>28/03/2025 03:46:18 PM</t>
   </si>
   <si>
     <t>Error Message -&gt; No such user found</t>
@@ -71,12 +71,21 @@
     <t>Invalid OTP Attempt</t>
   </si>
   <si>
-    <t>28/03/2025 03:19:22 PM</t>
+    <t>28/03/2025 03:46:21 PM</t>
   </si>
   <si>
     <t>Error Message -&gt; Incorrect OTP</t>
   </si>
   <si>
+    <t>Account Blocked After Multiple Wrong OTPs</t>
+  </si>
+  <si>
+    <t>28/03/2025 03:46:25 PM</t>
+  </si>
+  <si>
+    <t>You have reached the maximum login attempts for the day. Please try again after 24 hours.</t>
+  </si>
+  <si>
     <t>Click Go to Sign In</t>
   </si>
   <si>
@@ -84,6 +93,24 @@
   </si>
   <si>
     <t>User Login with Invalid Credentials</t>
+  </si>
+  <si>
+    <t>FAILED</t>
+  </si>
+  <si>
+    <t>28/03/2025 03:46:26 PM</t>
+  </si>
+  <si>
+    <t>stale element reference: stale element not found in the current frame
+  (Session info: chrome=134.0.6998.166)
+For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#stale-element-reference-exception
+Build info: version: '4.29.0', revision: '5fc1ec94cb'
+System info: os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '23.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Command: [f0be20835ff80e2a170a0b82c403494d, clickElement {id=f.00095D8C67BDCF3ABF05023232D37247.d.F5A6A02415C47404393A2FB587A4C4BE.e.31}]
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 134.0.6998.166, chrome: {chromedriverVersion: 134.0.6998.165 (fd886e2cb29..., userDataDir: C:\Users\Admin\AppData\Loca...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:58998}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:58998/devtoo..., se:cdpVersion: 134.0.6998.166, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Element: [[ChromeDriver: chrome on windows (f0be20835ff80e2a170a0b82c403494d)] -&gt; xpath: //button[@id='loginButton']]
+Session ID: f0be20835ff80e2a170a0b82c403494d</t>
   </si>
   <si>
     <t>Verify Home Page Loads Successfully</t>
@@ -137,7 +164,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -257,49 +284,69 @@
         <v>8</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n" s="0">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s" s="0">
         <v>8</v>
       </c>
       <c r="E7" t="s" s="0">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F7" t="s" s="0">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n" s="0">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s" s="0">
         <v>7</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s" s="0">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="F8" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="F9" t="s" s="0">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added methods to every steps
</commit_message>
<xml_diff>
--- a/test-output/TestReport.xlsx
+++ b/test-output/TestReport.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -41,7 +41,7 @@
     <t>PASSED</t>
   </si>
   <si>
-    <t>28/03/2025 03:46:14 PM</t>
+    <t>01/04/2025 01:11:31 PM</t>
   </si>
   <si>
     <t>Test executed successfully.</t>
@@ -50,70 +50,55 @@
     <t/>
   </si>
   <si>
-    <t>Invalid Email Attempt</t>
-  </si>
-  <si>
-    <t>28/03/2025 03:46:17 PM</t>
-  </si>
-  <si>
-    <t>Error Message -&gt; Invalid email address. Please enter a valid email</t>
-  </si>
-  <si>
-    <t>Not Registered Email Attempt</t>
-  </si>
-  <si>
-    <t>28/03/2025 03:46:18 PM</t>
-  </si>
-  <si>
-    <t>Error Message -&gt; No such user found</t>
-  </si>
-  <si>
-    <t>Invalid OTP Attempt</t>
-  </si>
-  <si>
-    <t>28/03/2025 03:46:21 PM</t>
-  </si>
-  <si>
-    <t>Error Message -&gt; Incorrect OTP</t>
-  </si>
-  <si>
-    <t>Account Blocked After Multiple Wrong OTPs</t>
-  </si>
-  <si>
-    <t>28/03/2025 03:46:25 PM</t>
-  </si>
-  <si>
-    <t>You have reached the maximum login attempts for the day. Please try again after 24 hours.</t>
-  </si>
-  <si>
-    <t>Click Go to Sign In</t>
-  </si>
-  <si>
-    <t>Navigated back to Get OTP page successfully</t>
-  </si>
-  <si>
-    <t>User Login with Invalid Credentials</t>
+    <t>01/04/2025 01:11:33 PM</t>
+  </si>
+  <si>
+    <t>Verify Login with Invalid Email</t>
+  </si>
+  <si>
+    <t>01/04/2025 01:11:36 PM</t>
+  </si>
+  <si>
+    <t>Verify Login with Not Registred Email</t>
+  </si>
+  <si>
+    <t>01/04/2025 01:11:37 PM</t>
+  </si>
+  <si>
+    <t>Verify Login with Invalid OTP</t>
+  </si>
+  <si>
+    <t>01/04/2025 01:11:39 PM</t>
+  </si>
+  <si>
+    <t>Verify account block after attempting wrong OTP for 5 times</t>
+  </si>
+  <si>
+    <t>01/04/2025 01:11:51 PM</t>
+  </si>
+  <si>
+    <t>Verify Go To Sign In page Navigation</t>
+  </si>
+  <si>
+    <t>01/04/2025 01:11:53 PM</t>
+  </si>
+  <si>
+    <t>Verify that navigation and getOTP blocked for blocked account</t>
+  </si>
+  <si>
+    <t>01/04/2025 01:11:54 PM</t>
+  </si>
+  <si>
+    <t>Verify Home Page Loads Successfully</t>
   </si>
   <si>
     <t>FAILED</t>
   </si>
   <si>
-    <t>28/03/2025 03:46:26 PM</t>
-  </si>
-  <si>
-    <t>stale element reference: stale element not found in the current frame
-  (Session info: chrome=134.0.6998.166)
-For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#stale-element-reference-exception
-Build info: version: '4.29.0', revision: '5fc1ec94cb'
-System info: os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '23.0.1'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Command: [f0be20835ff80e2a170a0b82c403494d, clickElement {id=f.00095D8C67BDCF3ABF05023232D37247.d.F5A6A02415C47404393A2FB587A4C4BE.e.31}]
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 134.0.6998.166, chrome: {chromedriverVersion: 134.0.6998.165 (fd886e2cb29..., userDataDir: C:\Users\Admin\AppData\Loca...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:58998}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:58998/devtoo..., se:cdpVersion: 134.0.6998.166, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
-Element: [[ChromeDriver: chrome on windows (f0be20835ff80e2a170a0b82c403494d)] -&gt; xpath: //button[@id='loginButton']]
-Session ID: f0be20835ff80e2a170a0b82c403494d</t>
-  </si>
-  <si>
-    <t>Verify Home Page Loads Successfully</t>
+    <t>01/04/2025 01:12:05 PM</t>
+  </si>
+  <si>
+    <t>Home Page did not load successfully. expected [true] but found [false]</t>
   </si>
 </sst>
 </file>
@@ -164,7 +149,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -218,124 +203,124 @@
         <v>11</v>
       </c>
       <c r="C3" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="D3" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>13</v>
-      </c>
       <c r="F3" t="s" s="0">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n" s="0">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s" s="0">
         <v>8</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n" s="0">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s" s="0">
         <v>8</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n" s="0">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s" s="0">
         <v>8</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>23</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n" s="0">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s" s="0">
         <v>8</v>
       </c>
       <c r="E7" t="s" s="0">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F7" t="s" s="0">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n" s="0">
-        <v>3.0</v>
+        <v>7.0</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s" s="0">
         <v>7</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="E8" t="s" s="0">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F8" t="s" s="0">
-        <v>29</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n" s="0">
-        <v>4.0</v>
+        <v>8.0</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s" s="0">
         <v>7</v>
@@ -344,10 +329,30 @@
         <v>8</v>
       </c>
       <c r="E9" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="F9" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n" s="0">
+        <v>9.0</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="F10" t="s" s="0">
         <v>28</v>
-      </c>
-      <c r="F9" t="s" s="0">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All working fine and updated
</commit_message>
<xml_diff>
--- a/test-output/TestReport.xlsx
+++ b/test-output/TestReport.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -35,7 +35,7 @@
     <t>PASSED</t>
   </si>
   <si>
-    <t>01/04/2025 01:30:37 PM</t>
+    <t>01/04/2025 01:36:14 PM</t>
   </si>
   <si>
     <t>Test executed successfully.</t>
@@ -44,13 +44,13 @@
     <t/>
   </si>
   <si>
-    <t>01/04/2025 01:30:39 PM</t>
+    <t>01/04/2025 01:36:16 PM</t>
   </si>
   <si>
     <t>Verify Login with Invalid Email</t>
   </si>
   <si>
-    <t>01/04/2025 01:30:40 PM</t>
+    <t>01/04/2025 01:36:17 PM</t>
   </si>
   <si>
     <t>Verify Login with Not Registred Email</t>
@@ -59,37 +59,28 @@
     <t>Verify Login with Invalid OTP</t>
   </si>
   <si>
-    <t>01/04/2025 01:30:43 PM</t>
+    <t>01/04/2025 01:36:20 PM</t>
   </si>
   <si>
     <t>Verify account block after attempting wrong OTP for 5 times</t>
   </si>
   <si>
-    <t>01/04/2025 01:30:55 PM</t>
+    <t>01/04/2025 01:36:32 PM</t>
   </si>
   <si>
     <t>Verify Go To Sign In page Navigation</t>
   </si>
   <si>
-    <t>01/04/2025 01:30:57 PM</t>
+    <t>01/04/2025 01:36:34 PM</t>
   </si>
   <si>
     <t>Verify that navigation and getOTP blocked for blocked account</t>
   </si>
   <si>
-    <t>01/04/2025 01:30:58 PM</t>
+    <t>01/04/2025 01:36:35 PM</t>
   </si>
   <si>
     <t>Verify Home Page Loads Successfully</t>
-  </si>
-  <si>
-    <t>FAILED</t>
-  </si>
-  <si>
-    <t>01/04/2025 01:31:09 PM</t>
-  </si>
-  <si>
-    <t>Home Page did not load successfully. expected [true] but found [false]</t>
   </si>
 </sst>
 </file>
@@ -307,13 +298,13 @@
         <v>22</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E10" t="s" s="0">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated testReportListener.java to exclude methods
</commit_message>
<xml_diff>
--- a/test-output/TestReport.xlsx
+++ b/test-output/TestReport.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -35,49 +35,46 @@
     <t>PASSED</t>
   </si>
   <si>
-    <t>01/04/2025 01:36:14 PM</t>
+    <t>01/04/2025 01:55:45 PM</t>
   </si>
   <si>
     <t>Test executed successfully.</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>01/04/2025 01:36:16 PM</t>
-  </si>
-  <si>
     <t>Verify Login with Invalid Email</t>
   </si>
   <si>
-    <t>01/04/2025 01:36:17 PM</t>
+    <t>01/04/2025 01:55:47 PM</t>
   </si>
   <si>
     <t>Verify Login with Not Registred Email</t>
   </si>
   <si>
+    <t>01/04/2025 01:55:48 PM</t>
+  </si>
+  <si>
     <t>Verify Login with Invalid OTP</t>
   </si>
   <si>
-    <t>01/04/2025 01:36:20 PM</t>
+    <t>01/04/2025 01:55:51 PM</t>
   </si>
   <si>
     <t>Verify account block after attempting wrong OTP for 5 times</t>
   </si>
   <si>
-    <t>01/04/2025 01:36:32 PM</t>
+    <t>01/04/2025 01:56:03 PM</t>
   </si>
   <si>
     <t>Verify Go To Sign In page Navigation</t>
   </si>
   <si>
-    <t>01/04/2025 01:36:34 PM</t>
+    <t>01/04/2025 01:56:05 PM</t>
   </si>
   <si>
     <t>Verify that navigation and getOTP blocked for blocked account</t>
   </si>
   <si>
-    <t>01/04/2025 01:36:35 PM</t>
+    <t>01/04/2025 01:56:06 PM</t>
   </si>
   <si>
     <t>Verify Home Page Loads Successfully</t>
@@ -131,7 +128,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -216,7 +213,7 @@
         <v>6</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s" s="0">
         <v>8</v>
@@ -227,13 +224,13 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s" s="0">
         <v>6</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s" s="0">
         <v>8</v>
@@ -244,13 +241,13 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s" s="0">
         <v>6</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s" s="0">
         <v>8</v>
@@ -261,13 +258,13 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s" s="0">
         <v>6</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s" s="0">
         <v>8</v>
@@ -278,32 +275,15 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C9" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="D9" t="s" s="0">
-        <v>21</v>
-      </c>
       <c r="E9" t="s" s="0">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n" s="0">
-        <v>9.0</v>
-      </c>
-      <c r="B10" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="D10" t="s" s="0">
-        <v>21</v>
-      </c>
-      <c r="E10" t="s" s="0">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
profile page id updated
</commit_message>
<xml_diff>
--- a/test-output/TestReport.xlsx
+++ b/test-output/TestReport.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -35,7 +35,7 @@
     <t>PASSED</t>
   </si>
   <si>
-    <t>22/04/2025 06:34:13 PM</t>
+    <t>13/05/2025 11:04:40 AM</t>
   </si>
   <si>
     <t>Test executed successfully.</t>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t>Navigate to Profile Page</t>
+  </si>
+  <si>
+    <t>13/05/2025 11:04:41 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Verify profile page loads</t>
   </si>
 </sst>
 </file>
@@ -95,7 +101,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -163,9 +169,26 @@
         <v>6</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s" s="0">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Login & Logout flow completed
</commit_message>
<xml_diff>
--- a/test-output/TestReport.xlsx
+++ b/test-output/TestReport.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -35,7 +35,7 @@
     <t>PASSED</t>
   </si>
   <si>
-    <t>13/05/2025 11:04:40 AM</t>
+    <t>14/05/2025 01:11:39 PM</t>
   </si>
   <si>
     <t>Test executed successfully.</t>
@@ -47,10 +47,19 @@
     <t>Navigate to Profile Page</t>
   </si>
   <si>
-    <t>13/05/2025 11:04:41 AM</t>
+    <t>14/05/2025 01:11:40 PM</t>
   </si>
   <si>
     <t xml:space="preserve"> Verify profile page loads</t>
+  </si>
+  <si>
+    <t>14/05/2025 01:11:41 PM</t>
+  </si>
+  <si>
+    <t>Logged out successfully</t>
+  </si>
+  <si>
+    <t>14/05/2025 01:11:42 PM</t>
   </si>
 </sst>
 </file>
@@ -101,7 +110,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -186,9 +195,26 @@
         <v>6</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s" s="0">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated with proffer working
</commit_message>
<xml_diff>
--- a/test-output/TestReport.xlsx
+++ b/test-output/TestReport.xlsx
@@ -35,7 +35,7 @@
     <t>PASSED</t>
   </si>
   <si>
-    <t>19/05/2025 05:19:08 PM</t>
+    <t>19/05/2025 06:00:16 PM</t>
   </si>
   <si>
     <t>Test executed successfully.</t>
@@ -44,31 +44,28 @@
     <t>Verify empty email state</t>
   </si>
   <si>
-    <t>19/05/2025 05:19:11 PM</t>
+    <t>19/05/2025 06:00:18 PM</t>
   </si>
   <si>
     <t>Verify Login with Invalid Email</t>
   </si>
   <si>
-    <t>19/05/2025 05:19:12 PM</t>
+    <t>19/05/2025 06:00:19 PM</t>
   </si>
   <si>
     <t>Verify Login with Not Registred Email</t>
   </si>
   <si>
-    <t>19/05/2025 05:19:13 PM</t>
+    <t>19/05/2025 06:00:20 PM</t>
   </si>
   <si>
     <t>Verify admin viewer Shouldn't be able to login</t>
   </si>
   <si>
-    <t>19/05/2025 05:19:14 PM</t>
-  </si>
-  <si>
     <t>Verify Login with Wrong OTP</t>
   </si>
   <si>
-    <t>19/05/2025 05:19:16 PM</t>
+    <t>19/05/2025 06:00:24 PM</t>
   </si>
   <si>
     <t>Verify same email on OTP page</t>
@@ -77,37 +74,37 @@
     <t>Verify account block after attempting wrong OTP for 5 times</t>
   </si>
   <si>
-    <t>19/05/2025 05:19:28 PM</t>
+    <t>19/05/2025 06:00:36 PM</t>
   </si>
   <si>
     <t>Verify Go To Sign In page Navigation</t>
   </si>
   <si>
-    <t>19/05/2025 05:19:31 PM</t>
+    <t>19/05/2025 06:00:38 PM</t>
   </si>
   <si>
     <t>Verify that navigation and getOTP blocked for blocked account</t>
   </si>
   <si>
+    <t>19/05/2025 06:00:39 PM</t>
+  </si>
+  <si>
     <t>Verify Resend OTP button</t>
   </si>
   <si>
+    <t>19/05/2025 06:01:43 PM</t>
+  </si>
+  <si>
+    <t>Verify account block after 5 times of resend otp</t>
+  </si>
+  <si>
     <t>FAILED</t>
   </si>
   <si>
-    <t>19/05/2025 05:20:36 PM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resend OTP failed: </t>
-  </si>
-  <si>
-    <t>Verify account block after 5 times of resend otp</t>
-  </si>
-  <si>
-    <t>SKIPPED</t>
-  </si>
-  <si>
-    <t>Test was skipped.</t>
+    <t>19/05/2025 06:04:57 PM</t>
+  </si>
+  <si>
+    <t>Error message isn't as expected expected [You have reached the maximum login attempts for the day. Please try again after 24 hours.] but found []</t>
   </si>
   <si>
     <t>Verify Home Page Loads Successfully</t>
@@ -116,16 +113,19 @@
     <t>Navigate to Profile Page</t>
   </si>
   <si>
+    <t>19/05/2025 06:04:58 PM</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Verify profile page loads</t>
   </si>
   <si>
-    <t>19/05/2025 05:20:37 PM</t>
+    <t>19/05/2025 06:04:59 PM</t>
   </si>
   <si>
     <t>Logged out successfully</t>
   </si>
   <si>
-    <t>19/05/2025 05:20:38 PM</t>
+    <t>19/05/2025 06:05:00 PM</t>
   </si>
 </sst>
 </file>
@@ -278,7 +278,7 @@
         <v>6</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s" s="0">
         <v>8</v>
@@ -289,13 +289,13 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s" s="0">
         <v>17</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s" s="0">
-        <v>18</v>
       </c>
       <c r="E7" t="s" s="0">
         <v>8</v>
@@ -306,13 +306,13 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s" s="0">
         <v>6</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s" s="0">
         <v>8</v>
@@ -323,13 +323,13 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s" s="0">
         <v>20</v>
-      </c>
-      <c r="C9" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="D9" t="s" s="0">
-        <v>21</v>
       </c>
       <c r="E9" t="s" s="0">
         <v>8</v>
@@ -340,13 +340,13 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s" s="0">
         <v>22</v>
-      </c>
-      <c r="C10" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="D10" t="s" s="0">
-        <v>23</v>
       </c>
       <c r="E10" t="s" s="0">
         <v>8</v>
@@ -357,13 +357,13 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s" s="0">
         <v>24</v>
-      </c>
-      <c r="C11" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="D11" t="s" s="0">
-        <v>23</v>
       </c>
       <c r="E11" t="s" s="0">
         <v>8</v>
@@ -377,13 +377,13 @@
         <v>25</v>
       </c>
       <c r="C12" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="D12" t="s" s="0">
-        <v>27</v>
-      </c>
       <c r="E12" t="s" s="0">
-        <v>28</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13">
@@ -391,16 +391,16 @@
         <v>12.0</v>
       </c>
       <c r="B13" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="C13" t="s" s="0">
+      <c r="E13" t="s" s="0">
         <v>30</v>
-      </c>
-      <c r="D13" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="E13" t="s" s="0">
-        <v>31</v>
       </c>
     </row>
     <row r="14">
@@ -408,13 +408,13 @@
         <v>13.0</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s" s="0">
         <v>6</v>
       </c>
       <c r="D14" t="s" s="0">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E14" t="s" s="0">
         <v>8</v>
@@ -425,13 +425,13 @@
         <v>14.0</v>
       </c>
       <c r="B15" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s" s="0">
         <v>33</v>
-      </c>
-      <c r="C15" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="D15" t="s" s="0">
-        <v>27</v>
       </c>
       <c r="E15" t="s" s="0">
         <v>8</v>

</xml_diff>

<commit_message>
Updated test report listener
</commit_message>
<xml_diff>
--- a/test-output/TestReport.xlsx
+++ b/test-output/TestReport.xlsx
@@ -35,7 +35,7 @@
     <t>PASSED</t>
   </si>
   <si>
-    <t>20/05/2025 01:58:33 PM</t>
+    <t>03/06/2025 01:52:49 PM</t>
   </si>
   <si>
     <t>Test executed successfully.</t>
@@ -47,7 +47,7 @@
     <t>SKIPPED</t>
   </si>
   <si>
-    <t>Test was skipped.</t>
+    <t>Skipping invalid login test as per config</t>
   </si>
   <si>
     <t>Verify Login with Invalid Email</t>
@@ -86,16 +86,16 @@
     <t>Navigate to Profile Page</t>
   </si>
   <si>
+    <t>03/06/2025 01:52:50 PM</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Verify profile page loads</t>
   </si>
   <si>
-    <t>20/05/2025 01:58:34 PM</t>
-  </si>
-  <si>
     <t>Logged out successfully</t>
   </si>
   <si>
-    <t>20/05/2025 01:58:35 PM</t>
+    <t>03/06/2025 01:52:51 PM</t>
   </si>
 </sst>
 </file>
@@ -156,7 +156,7 @@
     <col min="2" max="2" width="56.9609375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="8.4453125" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="23.53515625" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="25.09375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="35.59765625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -408,7 +408,7 @@
         <v>6</v>
       </c>
       <c r="D15" t="s" s="0">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="E15" t="s" s="0">
         <v>8</v>
@@ -419,13 +419,13 @@
         <v>15.0</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s" s="0">
         <v>6</v>
       </c>
       <c r="D16" t="s" s="0">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E16" t="s" s="0">
         <v>8</v>

</xml_diff>

<commit_message>
Added methods in empty state condition class
</commit_message>
<xml_diff>
--- a/test-output/TestReport.xlsx
+++ b/test-output/TestReport.xlsx
@@ -35,7 +35,7 @@
     <t>PASSED</t>
   </si>
   <si>
-    <t>03/06/2025 01:52:49 PM</t>
+    <t>04/06/2025 03:51:11 PM</t>
   </si>
   <si>
     <t>Test executed successfully.</t>
@@ -86,7 +86,7 @@
     <t>Navigate to Profile Page</t>
   </si>
   <si>
-    <t>03/06/2025 01:52:50 PM</t>
+    <t>04/06/2025 03:51:12 PM</t>
   </si>
   <si>
     <t xml:space="preserve"> Verify profile page loads</t>
@@ -95,7 +95,7 @@
     <t>Logged out successfully</t>
   </si>
   <si>
-    <t>03/06/2025 01:52:51 PM</t>
+    <t>04/06/2025 03:51:13 PM</t>
   </si>
 </sst>
 </file>

</xml_diff>